<commit_message>
Update values for 2050 and GaAs
</commit_message>
<xml_diff>
--- a/premise/data/metals/conversion_factors.xlsx
+++ b/premise/data/metals/conversion_factors.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92EDBA3-A497-824E-B0AC-53732DCFDE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D8D18F-61B1-4D87-B992-3611FC037CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3615" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conversion factors" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="162">
   <si>
     <t>Activity</t>
   </si>
@@ -717,6 +717,18 @@
   <si>
     <t xml:space="preserve">Battery energy density: 238 Wh/kg </t>
   </si>
+  <si>
+    <t>sputter process 1, perovskite cell</t>
+  </si>
+  <si>
+    <t>sputter process 2, perovskite cell</t>
+  </si>
+  <si>
+    <t>sputter process 3, perovskite cell</t>
+  </si>
+  <si>
+    <t>Conversion factor is one because I am taking an intensity of 0 for 2050, and want to use current values for the uncertainty</t>
+  </si>
 </sst>
 </file>
 
@@ -725,7 +737,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,6 +763,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -788,7 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -808,6 +827,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1091,21 +1111,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="171" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="61.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="33.5" customWidth="1"/>
-    <col min="5" max="5" width="49.33203125" customWidth="1"/>
-    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>151</v>
       </c>
@@ -1141,7 +1161,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>139</v>
       </c>
@@ -1157,7 +1177,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1179,7 +1199,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1200,7 +1220,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1221,7 +1241,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1242,7 +1262,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1262,7 +1282,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1282,7 +1302,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1303,7 +1323,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
@@ -1318,7 +1338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>150</v>
       </c>
@@ -1336,7 +1356,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -1357,7 +1377,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>79</v>
       </c>
@@ -1378,7 +1398,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>152</v>
       </c>
@@ -1396,7 +1416,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -1414,7 +1434,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>83</v>
       </c>
@@ -1435,7 +1455,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>86</v>
       </c>
@@ -1453,7 +1473,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>87</v>
       </c>
@@ -1474,7 +1494,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>88</v>
       </c>
@@ -1495,7 +1515,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>141</v>
       </c>
@@ -1512,7 +1532,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>89</v>
       </c>
@@ -1530,7 +1550,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>142</v>
       </c>
@@ -1550,7 +1570,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>154</v>
       </c>
@@ -1567,7 +1587,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>156</v>
       </c>
@@ -1585,7 +1605,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
         <v>143</v>
       </c>
@@ -1600,7 +1620,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>153</v>
       </c>
@@ -1615,7 +1635,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
         <v>144</v>
       </c>
@@ -1629,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
         <v>145</v>
       </c>
@@ -1643,7 +1663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>146</v>
       </c>
@@ -1657,7 +1677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
         <v>97</v>
       </c>
@@ -1675,7 +1695,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
         <v>98</v>
       </c>
@@ -1693,7 +1713,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>99</v>
       </c>
@@ -1711,7 +1731,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
         <v>100</v>
       </c>
@@ -1729,7 +1749,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
         <v>101</v>
       </c>
@@ -1747,7 +1767,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
         <v>102</v>
       </c>
@@ -1765,7 +1785,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
         <v>103</v>
       </c>
@@ -1783,7 +1803,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
         <v>104</v>
       </c>
@@ -1801,7 +1821,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
         <v>105</v>
       </c>
@@ -1819,7 +1839,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
         <v>106</v>
       </c>
@@ -1837,7 +1857,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
         <v>107</v>
       </c>
@@ -1855,7 +1875,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
         <v>108</v>
       </c>
@@ -1873,7 +1893,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
         <v>109</v>
       </c>
@@ -1891,7 +1911,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
         <v>110</v>
       </c>
@@ -1912,7 +1932,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
         <v>111</v>
       </c>
@@ -1926,7 +1946,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" s="1" t="s">
         <v>112</v>
       </c>
@@ -1940,7 +1960,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
         <v>113</v>
       </c>
@@ -1954,7 +1974,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
         <v>114</v>
       </c>
@@ -1968,7 +1988,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
@@ -1988,7 +2008,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
         <v>116</v>
       </c>
@@ -2002,7 +2022,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
         <v>117</v>
       </c>
@@ -2016,7 +2036,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" s="1" t="s">
         <v>118</v>
       </c>
@@ -2030,7 +2050,52 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="92" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="15.75">
+      <c r="A53" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15.75">
+      <c r="A54" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.75">
+      <c r="A55" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="8:8">
       <c r="H92">
         <f>SUM(H10:H85)</f>
         <v>0</v>
@@ -2053,13 +2118,13 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -2067,10 +2132,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -2085,7 +2150,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>207</v>
       </c>
@@ -2100,7 +2165,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>3750</v>
       </c>
@@ -2115,7 +2180,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>20</v>
       </c>
@@ -2130,7 +2195,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -2145,7 +2210,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>1460</v>
       </c>
@@ -2160,7 +2225,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>434</v>
       </c>
@@ -2175,7 +2240,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>14500</v>
       </c>
@@ -2190,7 +2255,7 @@
         <v>14500</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>207</v>
       </c>
@@ -2205,7 +2270,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>10230</v>
       </c>
@@ -2220,7 +2285,7 @@
         <v>10230</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>100</v>
       </c>
@@ -2235,7 +2300,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>621</v>
       </c>
@@ -2250,7 +2315,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>17510</v>
       </c>
@@ -2265,7 +2330,7 @@
         <v>17510</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>6480</v>
       </c>
@@ -2280,7 +2345,7 @@
         <v>6480</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>9660</v>
       </c>
@@ -2295,7 +2360,7 @@
         <v>9660</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>0.5</v>
       </c>
@@ -2310,7 +2375,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>1460</v>
       </c>
@@ -2325,7 +2390,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>14500</v>
       </c>
@@ -2340,7 +2405,7 @@
         <v>14500</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>-207</v>
       </c>
@@ -2355,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>-1.9250936128478799</v>
       </c>
@@ -2370,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>-0.1484134022501</v>
       </c>
@@ -2385,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>-6.13000504796797E-2</v>
       </c>
@@ -2400,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>-5.8210128804152599E-2</v>
       </c>
@@ -2415,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>-2.22122066071924</v>
       </c>
@@ -2430,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>-2.47645202667264E-2</v>
       </c>
@@ -2445,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>-1.12242641380724E-2</v>
       </c>
@@ -2460,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>-15.5497733604941</v>
       </c>
@@ -2475,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>10.2311999999993</v>
       </c>
@@ -2490,7 +2555,7 @@
         <v>10.2311999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>48.568800000000699</v>
       </c>
@@ -2505,7 +2570,7 @@
         <v>48.568800000000699</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>-6021.63645862063</v>
       </c>
@@ -2520,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>-7.6291978370255498</v>
       </c>
@@ -2535,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>-18700.734343542299</v>
       </c>
@@ -2550,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>-335.06254331617299</v>
       </c>
@@ -2565,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>-25.8313526616299</v>
       </c>
@@ -2580,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>-10.669273785988199</v>
       </c>
@@ -2595,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>-10.1314729183628</v>
       </c>
@@ -2610,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>-386.60345599818402</v>
       </c>
@@ -2625,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>-4.3102647524237199</v>
       </c>
@@ -2640,7 +2705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>-1.9535831732315101</v>
       </c>
@@ -2655,7 +2720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>-2706.4380533940098</v>
       </c>
@@ -2670,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>-59.774156678926602</v>
       </c>
@@ -2685,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>-4.6082361398656104</v>
       </c>
@@ -2700,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>-1.9033665673940501</v>
       </c>
@@ -2715,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>-1.8074244993689399</v>
       </c>
@@ -2730,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>-68.968901515332504</v>
       </c>
@@ -2745,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>-0.76893835428185298</v>
       </c>
@@ -2760,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>-0.34851340148714899</v>
       </c>
@@ -2775,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>-482.82046284334302</v>
       </c>
@@ -2790,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>-41.774531398798899</v>
       </c>
@@ -2805,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>-3.2205708288271699</v>
       </c>
@@ -2820,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>-1.33021109540905</v>
       </c>
@@ -2835,7 +2900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>-1.2631597950501099</v>
       </c>
@@ -2850,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>-48.200488337607602</v>
       </c>
@@ -2865,7 +2930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>-0.53739008978796199</v>
       </c>
@@ -2880,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>-0.24356653179617199</v>
       </c>
@@ -2895,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>-337.43008192272299</v>
       </c>
@@ -2910,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>-463.12334567726998</v>
       </c>
@@ -2925,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>-21.728740132701599</v>
       </c>
@@ -2940,7 +3005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>-975.14791419002802</v>
       </c>
@@ -2955,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>-955.84819645115397</v>
       </c>
@@ -2970,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>-46.379134770458698</v>
       </c>
@@ -2985,7 +3050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>-4.3271063444259603</v>
       </c>
@@ -3000,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>-19.362210571508601</v>
       </c>
@@ -3015,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>-503.20305355150998</v>
       </c>
@@ -3030,7 +3095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>-6.5709524492519602</v>
       </c>
@@ -3045,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>-1.0521864141291499</v>
       </c>
@@ -3060,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>-4742.2571594475603</v>
       </c>
@@ -3075,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>-16.140084415807301</v>
       </c>
@@ -3090,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>-0.39956428824000201</v>
       </c>
@@ -3105,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>-42.260351295952702</v>
       </c>
@@ -3120,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4">
       <c r="D73">
         <f>SUM(D4:D72)</f>
         <v>81198.799999999988</v>
@@ -3139,21 +3204,21 @@
       <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -3168,7 +3233,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>-1678</v>
       </c>
@@ -3183,7 +3248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>536.96</v>
       </c>
@@ -3198,7 +3263,7 @@
         <v>536.96</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>1141.04</v>
       </c>
@@ -3213,7 +3278,7 @@
         <v>1141.04</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>20688</v>
       </c>
@@ -3228,7 +3293,7 @@
         <v>20688</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>350</v>
       </c>
@@ -3243,7 +3308,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>2816</v>
       </c>
@@ -3258,7 +3323,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>144299.35</v>
       </c>
@@ -3273,7 +3338,7 @@
         <v>144299.35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>-440</v>
       </c>
@@ -3288,7 +3353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>440</v>
       </c>
@@ -3303,7 +3368,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>1646.57592</v>
       </c>
@@ -3318,7 +3383,7 @@
         <v>1646.57592</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>7816.5040799999997</v>
       </c>
@@ -3333,7 +3398,7 @@
         <v>7816.5040799999997</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>350</v>
       </c>
@@ -3348,7 +3413,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>14194.62</v>
       </c>
@@ -3363,7 +3428,7 @@
         <v>14194.62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>-20688</v>
       </c>
@@ -3378,7 +3443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>3088</v>
       </c>
@@ -3393,7 +3458,7 @@
         <v>3088</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>27000</v>
       </c>
@@ -3408,7 +3473,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>8000</v>
       </c>
@@ -3423,7 +3488,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>-1880.83323723227</v>
       </c>
@@ -3438,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>-893.25708316931002</v>
       </c>
@@ -3453,7 +3518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>-41.909679598416098</v>
       </c>
@@ -3468,7 +3533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>-158552.43309926699</v>
       </c>
@@ -3483,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>-51053.883457963901</v>
       </c>
@@ -3498,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>-64.683442769388705</v>
       </c>
@@ -3513,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>1678</v>
       </c>
@@ -3528,7 +3593,7 @@
         <v>1678</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>13328</v>
       </c>
@@ -3543,7 +3608,7 @@
         <v>13328</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>196140</v>
       </c>
@@ -3558,7 +3623,7 @@
         <v>196140</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>13328</v>
       </c>
@@ -3573,7 +3638,7 @@
         <v>13328</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>196140</v>
       </c>
@@ -3588,7 +3653,7 @@
         <v>196140</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>-5360.2913139542597</v>
       </c>
@@ -3603,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>-1080.4190098988299</v>
       </c>
@@ -3618,7 +3683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>-568.78293741068205</v>
       </c>
@@ -3633,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>-52.423490523606297</v>
       </c>
@@ -3648,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>-21.8855885827797</v>
       </c>
@@ -3663,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>-7.4273111208154896</v>
       </c>
@@ -3678,7 +3743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>-4.89103601359417</v>
       </c>
@@ -3693,7 +3758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>-1.18931249543923</v>
       </c>
@@ -3708,7 +3773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>-5518.0780984584399</v>
       </c>
@@ -3723,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>-788.23458037646503</v>
       </c>
@@ -3738,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>-683.14930747006804</v>
       </c>
@@ -3753,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>-52.666796196182901</v>
       </c>
@@ -3768,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>-21.753273063496799</v>
       </c>
@@ -3783,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>-20.656766463149999</v>
       </c>
@@ -3798,7 +3863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>-8.7880738667119793</v>
       </c>
@@ -3813,7 +3878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>-3.9831041054891401</v>
       </c>
@@ -3828,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>-2400.8850068603001</v>
       </c>
@@ -3843,7 +3908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>-342.95647001505102</v>
       </c>
@@ -3858,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>-297.23445382371199</v>
       </c>
@@ -3873,7 +3938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>-22.915029307415399</v>
       </c>
@@ -3888,7 +3953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>-9.4647277940625401</v>
       </c>
@@ -3903,7 +3968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>-8.9876438873611608</v>
       </c>
@@ -3918,7 +3983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>-3.8236419291825499</v>
       </c>
@@ -3933,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>-1.7330263829183801</v>
       </c>
@@ -3948,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>-6729.0976909670799</v>
       </c>
@@ -3963,7 +4028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>-2654.3326476308398</v>
       </c>
@@ -3978,7 +4043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>-79.64966140208</v>
       </c>
@@ -3993,7 +4058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>-809666.73499999999</v>
       </c>
@@ -4008,7 +4073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>-56732.144999999997</v>
       </c>
@@ -4023,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>-601.12</v>
       </c>
@@ -4038,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>296</v>
       </c>
@@ -4053,7 +4118,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>2816</v>
       </c>
@@ -4068,7 +4133,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>203</v>
       </c>
@@ -4083,7 +4148,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>979.68</v>
       </c>
@@ -4098,7 +4163,7 @@
         <v>979.68</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="D66">
         <f>SUM(D4:D65)</f>
         <v>657275.7300000001</v>
@@ -4117,21 +4182,21 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -4146,7 +4211,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="D4">
         <f>IF(A4&gt;0,A4,0)</f>
         <v>0</v>
@@ -4165,21 +4230,21 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -4194,7 +4259,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="D4">
         <f>IF(A4&gt;0,A4,0)</f>
         <v>0</v>

</xml_diff>